<commit_message>
Add charts to the slides.
Signed-off-by: Nikhil Nanivadekar <nikhil.nanivadekar@bnymellon.com>
</commit_message>
<xml_diff>
--- a/Person_Dataset_Multimap_based_Comparison.xlsx
+++ b/Person_Dataset_Multimap_based_Comparison.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\IntelliJ_Workspace\performance-reconciler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC44EAEC-D7D9-4AD2-9BC2-D82DA666A1A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A45FFE2A-0FCA-4F07-9974-E63032B41583}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="6" xr2:uid="{01B5B808-35CD-446D-B496-2DBD45D6B974}"/>
   </bookViews>
@@ -96,8 +96,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -19935,14 +19938,20 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4252613F-ED58-48A2-BB61-B78A2A3B24D2}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:U1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+    <sheetView topLeftCell="A24" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection sqref="A1:U1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="21" width="8.83984375" style="1"/>
+  </cols>
   <sheetData/>
+  <mergeCells count="1">
+    <mergeCell ref="A1:U1048576"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -19952,12 +19961,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29B8A951-4776-42BC-9BE5-32BC75520CA5}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="16384" width="8.83984375" style="1"/>
+  </cols>
   <sheetData/>
+  <mergeCells count="1">
+    <mergeCell ref="A1:XFD1048576"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Fix missing data for Person data set JDK-8
Signed-off-by: Nikhil Nanivadekar <nikhil.nanivadekar@bnymellon.com>
</commit_message>
<xml_diff>
--- a/Person_Dataset_Multimap_based_Comparison.xlsx
+++ b/Person_Dataset_Multimap_based_Comparison.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\IntelliJ_Workspace\performance-reconciler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A45FFE2A-0FCA-4F07-9974-E63032B41583}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7A32DA4-F432-4BBB-8275-63EBAB73B923}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="6" xr2:uid="{01B5B808-35CD-446D-B496-2DBD45D6B974}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="5" xr2:uid="{01B5B808-35CD-446D-B496-2DBD45D6B974}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2106,6 +2106,28 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-4.4044040572537848E-3"/>
+                  <c:y val="0"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-95A4-4251-97C2-2BB92B7FF4F1}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -2165,17 +2187,10 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                  <c15:fullRef>
-                    <c15:sqref>'JDK8-Memory'!$A$23:$A$27</c15:sqref>
-                  </c15:fullRef>
-                </c:ext>
-              </c:extLst>
-              <c:f>'JDK8-Memory'!$A$23:$A$26</c:f>
+              <c:f>'JDK8-Memory'!$A$23:$A$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
                 </c:pt>
@@ -2187,23 +2202,19 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                  <c15:fullRef>
-                    <c15:sqref>'JDK8-Memory'!$B$23:$B$27</c15:sqref>
-                  </c15:fullRef>
-                </c:ext>
-              </c:extLst>
-              <c:f>'JDK8-Memory'!$B$23:$B$26</c:f>
+              <c:f>'JDK8-Memory'!$B$23:$B$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>33.479999999999997</c:v>
                 </c:pt>
@@ -2215,6 +2226,9 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>38.51</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>318.44</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2250,6 +2264,28 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="1.9819818257642032E-2"/>
+                  <c:y val="3.1511395711670935E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-95A4-4251-97C2-2BB92B7FF4F1}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -2309,17 +2345,10 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                  <c15:fullRef>
-                    <c15:sqref>'JDK8-Memory'!$A$23:$A$27</c15:sqref>
-                  </c15:fullRef>
-                </c:ext>
-              </c:extLst>
-              <c:f>'JDK8-Memory'!$A$23:$A$26</c:f>
+              <c:f>'JDK8-Memory'!$A$23:$A$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
                 </c:pt>
@@ -2331,23 +2360,19 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                  <c15:fullRef>
-                    <c15:sqref>'JDK8-Memory'!$C$23:$C$27</c15:sqref>
-                  </c15:fullRef>
-                </c:ext>
-              </c:extLst>
-              <c:f>'JDK8-Memory'!$C$23:$C$26</c:f>
+              <c:f>'JDK8-Memory'!$C$23:$C$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>28.51</c:v>
                 </c:pt>
@@ -2359,6 +2384,9 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>43.99</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>320.61</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -18436,8 +18464,8 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>327660</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>346710</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>36195</xdr:rowOff>
     </xdr:from>
@@ -19659,7 +19687,7 @@
   <dimension ref="A22:C28"/>
   <sheetViews>
     <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="R33" sqref="R33"/>
+      <selection activeCell="N30" sqref="N30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -19940,7 +19968,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4252613F-ED58-48A2-BB61-B78A2A3B24D2}">
   <dimension ref="A1:U1"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection sqref="A1:U1048576"/>
     </sheetView>
   </sheetViews>
@@ -19961,7 +19989,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29B8A951-4776-42BC-9BE5-32BC75520CA5}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView topLeftCell="A23" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>

</xml_diff>